<commit_message>
Implement nicolas comments on the EN output
</commit_message>
<xml_diff>
--- a/input/ocha_pop_BFA.xlsx
+++ b/input/ocha_pop_BFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="370" documentId="13_ncr:1_{59E61301-DE0E-4AD8-9E51-0BB6543F4157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0DC4B8A-2C34-4301-BCAF-F8CD83A1437A}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="13_ncr:1_{59E61301-DE0E-4AD8-9E51-0BB6543F4157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CE53973-9A8B-4430-A5BC-8E3A796E752E}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ocha" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ocha!$A$1:$O$289</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'scope-fix'!$A$1:$C$352</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -14199,7 +14200,7 @@
   <dimension ref="A1:C352"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14209,7 +14210,7 @@
     <col min="3" max="3" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="131.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
@@ -16507,15 +16508,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" xsi:nil="true"/>
@@ -16524,6 +16516,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16546,14 +16547,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACDE1998-78A0-4AB1-AFCD-9276514F0C55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -16568,4 +16561,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>